<commit_message>
Grouping data in objects and allowing them to be written as a csv line
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HEIG-VD\2eme\RES\Teaching-HEIGVD-RES\examples\01-BufferedIOBenchmark\BufferedIOBenchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HEIG-VD\2eme\2eme semestre\RES\Teaching-HEIGVD-RES\examples\01-BufferedIOBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -987,11 +987,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427271024"/>
-        <c:axId val="427267104"/>
+        <c:axId val="317514240"/>
+        <c:axId val="317515416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427271024"/>
+        <c:axId val="317514240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1033,7 +1033,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-CH"/>
-                  <a:t>block size</a:t>
+                  <a:t>Block size</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1105,12 +1105,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427267104"/>
+        <c:crossAx val="317515416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427267104"/>
+        <c:axId val="317515416"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1152,11 +1152,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-CH"/>
-                  <a:t>time</a:t>
+                  <a:t>Duration </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="fr-CH" baseline="0"/>
-                  <a:t> taken [ms]</a:t>
+                  <a:t>[ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1228,7 +1228,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427271024"/>
+        <c:crossAx val="317514240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1702,7 +1702,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1710,11 +1709,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427277296"/>
-        <c:axId val="427268672"/>
+        <c:axId val="317511104"/>
+        <c:axId val="317516592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427277296"/>
+        <c:axId val="317511104"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1736,6 +1735,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>Block size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -1803,12 +1827,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427268672"/>
+        <c:crossAx val="317516592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427268672"/>
+        <c:axId val="317516592"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1830,6 +1854,35 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>Duration</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CH" baseline="0"/>
+                  <a:t> [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -1897,7 +1950,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427277296"/>
+        <c:crossAx val="317511104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3421,7 +3474,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>